<commit_message>
edits to excel files and adding in tables with sample data
</commit_message>
<xml_diff>
--- a/Excel Files for Table/House.xlsx
+++ b/Excel Files for Table/House.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anime\FinalProject\Excel Files for Table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{749F2E1C-FB55-4E48-91A4-9876F03ED6BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{618D1B03-3624-4228-A300-64911B91FEC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="1344" windowWidth="12216" windowHeight="10620" xr2:uid="{00856646-A83D-40E3-AAEE-08456134B45A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00856646-A83D-40E3-AAEE-08456134B45A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -446,8 +446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7FAA943-84BD-469F-9656-9B1FD1DC9B2F}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
switching utilities and adding basement
</commit_message>
<xml_diff>
--- a/Excel Files for Table/House.xlsx
+++ b/Excel Files for Table/House.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anime\FinalProject\Excel Files for Table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{618D1B03-3624-4228-A300-64911B91FEC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C5B2C33-1F69-4DE2-BB71-371599B352AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00856646-A83D-40E3-AAEE-08456134B45A}"/>
   </bookViews>
@@ -62,12 +62,6 @@
     <t>Bedrooms</t>
   </si>
   <si>
-    <t>tenant</t>
-  </si>
-  <si>
-    <t>landlord</t>
-  </si>
-  <si>
     <t>Bathrooms</t>
   </si>
   <si>
@@ -77,9 +71,6 @@
     <t>no</t>
   </si>
   <si>
-    <t>utilities</t>
-  </si>
-  <si>
     <t>Address</t>
   </si>
   <si>
@@ -93,6 +84,15 @@
   </si>
   <si>
     <t>Postal Code</t>
+  </si>
+  <si>
+    <t>basement</t>
+  </si>
+  <si>
+    <t>finished</t>
+  </si>
+  <si>
+    <t>unfinished</t>
   </si>
 </sst>
 </file>
@@ -447,12 +447,13 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="5" width="10.6640625" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="32.109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -470,19 +471,19 @@
         <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -502,13 +503,13 @@
         <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="H2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I2">
         <v>19103</v>
@@ -531,13 +532,13 @@
         <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="H3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I3">
         <v>19136</v>
@@ -560,13 +561,13 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G4" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="H4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I4">
         <v>19154</v>

</xml_diff>